<commit_message>
add flag to determine wating period for next analysis
</commit_message>
<xml_diff>
--- a/dataset/all.xlsx
+++ b/dataset/all.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W53"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,17 +543,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>05/04/2021 00:02:33</t>
+          <t>05/05/2021 01:39:46</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3390000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="C2" t="n">
-        <v>14.08</v>
+        <v>15.666</v>
       </c>
       <c r="D2" t="n">
-        <v>13.02</v>
+        <v>13.99</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -634,17 +634,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>05/04/2021 00:03:34</t>
+          <t>05/05/2021 01:40:48</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3390000000000001</v>
+        <v>0.3333</v>
       </c>
       <c r="C3" t="n">
-        <v>15.571</v>
+        <v>14.31</v>
       </c>
       <c r="D3" t="n">
-        <v>15.39</v>
+        <v>12.964</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -654,11 +654,6 @@
       </c>
       <c r="I3" t="n">
         <v>0</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>(0, 0, 0)</t>
-        </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -715,17 +710,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>05/04/2021 00:04:36</t>
+          <t>05/05/2021 01:41:50</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3390000000000001</v>
+        <v>0.3333</v>
       </c>
       <c r="C4" t="n">
-        <v>15.571</v>
+        <v>15.114</v>
       </c>
       <c r="D4" t="n">
-        <v>15.39</v>
+        <v>13.814</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -761,7 +756,7 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>(0, 0, 0)</t>
+          <t>(1, 0, 0)</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -784,7 +779,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>(0, 0, 0)</t>
+          <t>(1, 0, 0)</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -806,17 +801,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>05/04/2021 00:05:38</t>
+          <t>05/05/2021 01:42:55</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>0.3390000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>15.731</v>
+        <v>15.114</v>
       </c>
       <c r="D5" t="n">
-        <v>15.518</v>
+        <v>13.814</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -825,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>100</v>
+        <v>99.80141284210697</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -834,44 +829,44 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.33900000000000013</t>
+          <t>0.38886666607421916</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>0.33900000000000013</t>
+          <t>0.38886666607421916</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.33900000000000013</t>
+          <t>0.38886666607421916</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>99.95517893338445</v>
+        <v>0</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>(0, 0, 0)</t>
+          <t>(1, 0, 0)</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>15.074000000000002</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>15.074000000000002</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>15.074000000000002</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S5" t="n">
-        <v>99.93192242072151</v>
+        <v>99.97967038254413</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
@@ -880,34 +875,34 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>14.600000000000003</t>
+          <t>13.589333332583431</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>14.600000000000003</t>
+          <t>13.589333332583431</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>14.600000000000003</t>
+          <t>13.589333332583431</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05/04/2021 00:06:41</t>
+          <t>05/05/2021 01:44:00</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.3390000000000001</v>
+        <v>0.3279</v>
       </c>
       <c r="C6" t="n">
-        <v>15.731</v>
+        <v>14.95</v>
       </c>
       <c r="D6" t="n">
-        <v>15.518</v>
+        <v>13.862</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -916,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>100</v>
+        <v>99.85249487186034</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -925,44 +920,44 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.3390000000000001</t>
+          <t>0.3763999993002544</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>0.3390000000000001</t>
+          <t>0.3763999993002544</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0.3390000000000001</t>
+          <t>0.3763999993002544</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>99.96345591498799</v>
+        <v>99.980637029574</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>(0, 0, 0)</t>
+          <t>(1, 0, 0)</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>15.238249997352295</t>
+          <t>14.835321139022042</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>15.238249997352295</t>
+          <t>15.05023569880391</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>15.238249997352295</t>
+          <t>14.88449557827899</t>
         </is>
       </c>
       <c r="S6" t="n">
-        <v>99.94823753060962</v>
+        <v>99.9840590343162</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
@@ -971,34 +966,34 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>14.8295</t>
+          <t>13.645499992105938</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>14.8295</t>
+          <t>13.645499992105938</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>14.8295</t>
+          <t>13.645499992105938</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>05/04/2021 00:07:40</t>
+          <t>05/05/2021 01:45:04</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3390000000000001</v>
+        <v>43.5593</v>
       </c>
       <c r="C7" t="n">
-        <v>15.418</v>
+        <v>14.798</v>
       </c>
       <c r="D7" t="n">
-        <v>15.313</v>
+        <v>54.964</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -1007,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>100</v>
+        <v>99.57113605087845</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1016,44 +1011,44 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0.33899999999999997</t>
+          <t>0.36669999943701725</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>0.33899999999999997</t>
+          <t>0.36669999943701725</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0.33899999999999997</t>
+          <t>0.36669999943701725</t>
         </is>
       </c>
       <c r="N7" t="n">
-        <v>99.97388175281208</v>
+        <v>99.98278706171043</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>(0, 0, 0)</t>
+          <t>(1, 0, 0)</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>15.3368</t>
+          <t>14.989084709699082</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>15.3368</t>
+          <t>14.958670680259566</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>15.3368</t>
+          <t>14.9823375616019</t>
         </is>
       </c>
       <c r="S7" t="n">
-        <v>99.9579643138657</v>
+        <v>99.73905611868396</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
@@ -1062,34 +1057,34 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>14.967200002226118</t>
+          <t>13.688799997723356</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>14.967200002226118</t>
+          <t>13.688799997723356</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>14.967200002226118</t>
+          <t>13.688799997723356</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>05/04/2021 00:08:43</t>
+          <t>05/05/2021 01:46:09</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>31.3115</v>
+        <v>72.66670000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>19.465</v>
+        <v>18.395</v>
       </c>
       <c r="D8" t="n">
-        <v>59.218</v>
+        <v>66.68300000000001</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -1098,30 +1093,30 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>99.67027556435602</v>
+        <v>98.92424619044719</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>(0, 0, 0)</t>
+          <t>(2, 0, 0)</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.3390000000000002</t>
+          <t>-75.26268082991756</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>0.3390000000000002</t>
+          <t>119.14796193686945</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.3390000000000002</t>
+          <t>-150.84889400937357</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>99.91734065517312</v>
+        <v>99.93083878968133</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1130,57 +1125,57 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>15.350333331234951</t>
+          <t>14.991999999533457</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>15.350333331234951</t>
+          <t>14.991999999533457</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>15.350333331234951</t>
+          <t>14.991999999533457</t>
         </is>
       </c>
       <c r="S8" t="n">
-        <v>99.72892358834001</v>
+        <v>99.48338580856245</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>(0, 0, 0)</t>
+          <t>(1, 0, 0)</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>15.024833333333337</t>
+          <t>15.49793529195583</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>15.024833333333337</t>
+          <t>20.600294619451212</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>15.024833333333337</t>
+          <t>19.9406374963134</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>05/04/2021 00:09:46</t>
+          <t>05/05/2021 01:51:31</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49.4915</v>
+        <v>51.01690000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>19.465</v>
+        <v>38.542</v>
       </c>
       <c r="D9" t="n">
-        <v>59.218</v>
+        <v>133.993</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1193,7 +1188,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>(1, 0, 1)</t>
+          <t>(5,1,0)</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1212,66 +1207,66 @@
         </is>
       </c>
       <c r="N9" t="n">
-        <v>99.84839313937933</v>
+        <v>99.73362126871584</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
+          <t>(0, 0, 0)</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>15.478142850915033</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>15.478142850915033</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>15.478142850915033</t>
+        </is>
+      </c>
+      <c r="S9" t="n">
+        <v>99.30147198489153</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
           <t>(1, 0, 0)</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>14.830761183151093</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>16.187774630611774</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>15.790409374014736</t>
-        </is>
-      </c>
-      <c r="S9" t="n">
-        <v>99.33907062032509</v>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>(0, 0, 1)</t>
-        </is>
-      </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>-10.742637778989714</t>
+          <t>56.96606347134888</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>18.881071852118534</t>
+          <t>50.023519098738774</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>18.881071852118534</t>
+          <t>45.06321888235451</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05/04/2021 00:10:51</t>
+          <t>05/05/2021 01:52:37</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>69.3443</v>
+        <v>30.83335</v>
       </c>
       <c r="C10" t="n">
-        <v>19.297</v>
+        <v>19.865</v>
       </c>
       <c r="D10" t="n">
-        <v>118.654</v>
+        <v>79.185</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1280,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>98.90312268056391</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -1289,80 +1284,80 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.8512509181298142</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-38.022290376879546</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>-34.75641770302582</t>
         </is>
       </c>
       <c r="N10" t="n">
-        <v>99.87469988345629</v>
+        <v>99.78128976225925</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
+          <t>(0, 0, 0)</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>18.361124999999998</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>18.361124999999998</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>18.361124999999998</t>
+        </is>
+      </c>
+      <c r="S10" t="n">
+        <v>99.34644594254387</v>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
           <t>(1, 0, 0)</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>18.402007372415422</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>17.72018818819458</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>17.282859284956643</t>
-        </is>
-      </c>
-      <c r="S10" t="n">
-        <v>99.47529177227658</v>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>(1, 0, 0)</t>
-        </is>
-      </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>48.69494127022378</t>
+          <t>120.25288952956124</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>41.86670986042947</t>
+          <t>109.00558024811326</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>37.43598820591931</t>
+          <t>99.79881540115592</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>05/04/2021 00:11:57</t>
+          <t>05/05/2021 01:53:43</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>72.5424</v>
+        <v>54.9863</v>
       </c>
       <c r="C11" t="n">
-        <v>20.086</v>
+        <v>37.938</v>
       </c>
       <c r="D11" t="n">
-        <v>118.654</v>
+        <v>189.745</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -1371,89 +1366,89 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>99.48417809016419</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>(2, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>22.39119064521762</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>20.932291120618842</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>20.932291120618842</t>
         </is>
       </c>
       <c r="N11" t="n">
-        <v>99.85732026499795</v>
+        <v>99.65731813327325</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>18.588476568676377</t>
+          <t>18.52822222222222</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>18.07308727688858</t>
+          <t>18.52822222222222</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>17.698186306297806</t>
+          <t>18.52822222222222</t>
         </is>
       </c>
       <c r="S11" t="n">
-        <v>99.45382399390255</v>
+        <v>0</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(5,1,0)</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>105.60345692426961</t>
+          <t>0</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>95.0560886370343</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>86.53177074918649</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>05/04/2021 00:17:15</t>
+          <t>05/05/2021 01:54:50</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>51.14265</v>
+        <v>22.13115</v>
       </c>
       <c r="C12" t="n">
-        <v>40.36199999999999</v>
+        <v>19.284</v>
       </c>
       <c r="D12" t="n">
-        <v>136.36</v>
+        <v>66.16</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -1462,30 +1457,30 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>99.46142462140354</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>(2, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>52.975924520416385</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>26.375624039607317</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>26.375624039607317</t>
         </is>
       </c>
       <c r="N12" t="n">
-        <v>99.73034921005859</v>
+        <v>99.68820204449321</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1494,57 +1489,57 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>17.04150002400281</t>
+          <t>20.4692</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>17.04150002400281</t>
+          <t>20.4692</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>17.04150002400281</t>
+          <t>20.4692</t>
         </is>
       </c>
       <c r="S12" t="n">
-        <v>99.5917540845267</v>
+        <v>0</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(5,1,0)</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>109.83000821696888</t>
+          <t>0</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>102.25359208285693</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>95.74836374077955</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>05/04/2021 00:18:24</t>
+          <t>05/05/2021 02:00:08</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>50.04235</v>
+        <v>68.66670000000001</v>
       </c>
       <c r="C13" t="n">
-        <v>41.998</v>
+        <v>18.601</v>
       </c>
       <c r="D13" t="n">
-        <v>152.163</v>
+        <v>65.178</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1553,89 +1548,89 @@
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>99.43157172600459</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>(2, 0, 0)</t>
+          <t>(1, 0, 0)</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>22.17014791096265</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>22.19348308203964</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>22.207446143028065</t>
         </is>
       </c>
       <c r="N13" t="n">
-        <v>99.78761456805513</v>
+        <v>99.73163303449296</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>34.18691384416231</t>
+          <t>20.36145454545454</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>30.019575615339928</t>
+          <t>20.36145454545454</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>27.207192520573436</t>
+          <t>20.36145454545454</t>
         </is>
       </c>
       <c r="S13" t="n">
-        <v>99.8493651758312</v>
+        <v>0</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>(0, 1, 0)</t>
+          <t>(5,1,0)</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>148.69400000000002</t>
+          <t>0</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>161.02800000000002</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>173.36200000000002</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>05/04/2021 00:19:32</t>
+          <t>05/05/2021 02:01:17</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>62.57925</v>
+        <v>89.16670000000001</v>
       </c>
       <c r="C14" t="n">
-        <v>41.998</v>
+        <v>18.398</v>
       </c>
       <c r="D14" t="n">
-        <v>152.163</v>
+        <v>111.654</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -1644,89 +1639,89 @@
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>99.23526399894631</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>(1, 0, 1)</t>
+          <t>(0, 1, 0)</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>74.86367272727273</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>81.06064545454545</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>87.25761818181817</t>
         </is>
       </c>
       <c r="N14" t="n">
-        <v>99.82187968411344</v>
+        <v>99.83156528830138</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>39.19442281638063</t>
+          <t>20.214750000000006</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>36.83586484913961</t>
+          <t>20.214750000000006</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>34.851687021848754</t>
+          <t>20.214750000000006</t>
         </is>
       </c>
       <c r="S14" t="n">
-        <v>99.85874358605719</v>
+        <v>0</v>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>(0, 1, 0)</t>
+          <t>(5,1,0)</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>164.81236363636364</t>
+          <t>0</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>177.46172727272727</t>
+          <t>0</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>190.1110909090909</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>05/04/2021 00:36:09</t>
+          <t>05/05/2021 02:06:33</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.33335</v>
+        <v>30.25</v>
       </c>
       <c r="C15" t="n">
-        <v>27.71</v>
+        <v>105687.46</v>
       </c>
       <c r="D15" t="n">
-        <v>25.404</v>
+        <v>622.159</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1735,89 +1730,89 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>64.57849463834191</v>
+        <v>99.21487133363145</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>59.119814956747</t>
+          <t>48.169205039469375</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>56.03652367992327</t>
+          <t>33.52239884362161</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>53.28847812367606</t>
+          <t>33.52239884362161</t>
         </is>
       </c>
       <c r="N15" t="n">
-        <v>99.74317035155359</v>
+        <v>99.64674422909327</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>39.90036462047675</t>
+          <t>20.07500000000001</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>38.06840356711392</t>
+          <t>20.07500000000001</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>36.46846807126953</t>
+          <t>20.07500000000001</t>
         </is>
       </c>
       <c r="S15" t="n">
-        <v>98.94047868553017</v>
+        <v>99.2039988885825</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 1, 0)</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>147.6070235281048</t>
+          <t>119.79266666666666</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>143.33200380259643</t>
+          <t>127.93133333333333</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>139.3206148574987</t>
+          <t>136.07</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>05/04/2021 00:38:19</t>
+          <t>05/05/2021 02:07:38</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>77</v>
+        <v>0.3333</v>
       </c>
       <c r="C16" t="n">
-        <v>18.743</v>
+        <v>28.264</v>
       </c>
       <c r="D16" t="n">
-        <v>64.738</v>
+        <v>25.656</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1826,89 +1821,89 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>88.9141893443399</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>(2, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>21.19428722668588</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>31.499901531381585</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>31.499901531381585</t>
         </is>
       </c>
       <c r="N16" t="n">
-        <v>99.77440763239105</v>
+        <v>55.24693684140368</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>(2, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>20.423587186921623</t>
+          <t>7567.745357142859</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>18.226138968913457</t>
+          <t>7567.745357142859</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>18.64996157146064</t>
+          <t>7567.745357142859</t>
         </is>
       </c>
       <c r="S16" t="n">
-        <v>99.03579762074592</v>
+        <v>99.10603483302719</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>33.17125251183796</t>
+          <t>104.15464285714287</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>38.74510314961606</t>
+          <t>104.15464285714287</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>42.74494876875992</t>
+          <t>104.15464285714287</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>05/04/2021 00:43:40</t>
+          <t>05/05/2021 02:12:49</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>51.4167</v>
+        <v>0.5</v>
       </c>
       <c r="C17" t="n">
-        <v>37.718</v>
+        <v>14.396</v>
       </c>
       <c r="D17" t="n">
-        <v>139.532</v>
+        <v>12.944</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1917,89 +1912,89 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>70.32982287822587</v>
+        <v>83.67006492217467</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>56.40290157645322</t>
+          <t>16.528766271251236</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>45.25233469809561</t>
+          <t>29.321542899822397</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>39.21579794170547</t>
+          <t>29.321542899822397</t>
         </is>
       </c>
       <c r="N17" t="n">
-        <v>99.6336560511553</v>
+        <v>-26.29599184932783</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>(0, 1, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>19.076071428571428</t>
+          <t>7065.113266666667</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>19.409142857142857</t>
+          <t>7065.113266666667</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>19.742214285714287</t>
+          <t>7065.113266666667</t>
         </is>
       </c>
       <c r="S17" t="n">
-        <v>98.96270236054306</v>
+        <v>98.12630054635223</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>62.99035564310718</t>
+          <t>98.9214</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>61.77913584878266</t>
+          <t>98.9214</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>60.939689662619344</t>
+          <t>98.9214</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>05/04/2021 00:44:48</t>
+          <t>05/05/2021 02:13:53</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>51.15575</v>
+        <v>0.3390000000000001</v>
       </c>
       <c r="C18" t="n">
-        <v>37.718</v>
+        <v>14.638</v>
       </c>
       <c r="D18" t="n">
-        <v>139.532</v>
+        <v>13.124</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -2008,89 +2003,89 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>75.2769301046702</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>(2, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>17.883109568016465</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>27.70957689146774</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>27.70957689146774</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>99.70766267898708</v>
+        <v>-101.5442700971687</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>(0, 1, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>39.29386666666667</t>
+          <t>6624.443437500003</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>40.86973333333334</t>
+          <t>6624.443437500003</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>42.44560000000001</t>
+          <t>6624.443437500003</t>
         </is>
       </c>
       <c r="S18" t="n">
-        <v>98.88083895388091</v>
+        <v>97.12224577999841</v>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>(0, 1, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>147.96613333333335</t>
+          <t>93.54781250000003</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>156.40026666666668</t>
+          <t>93.54781250000003</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>164.83440000000002</t>
+          <t>93.54781250000003</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>05/04/2021 00:50:03</t>
+          <t>05/05/2021 02:14:57</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.3333</v>
+        <v>0.3390000000000001</v>
       </c>
       <c r="C19" t="n">
-        <v>14.218</v>
+        <v>16.392</v>
       </c>
       <c r="D19" t="n">
-        <v>12.916</v>
+        <v>15.232</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -2099,89 +2094,89 @@
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>56.48150168351794</v>
+        <v>72.69551319086213</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>42.58985771084153</t>
+          <t>14.845823030983341</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>37.95687565499715</t>
+          <t>26.058784621612617</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>35.451062833028466</t>
+          <t>26.058784621612617</t>
         </is>
       </c>
       <c r="N19" t="n">
-        <v>99.65795944090502</v>
+        <v>-126.9532298467712</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>(0, 0, 1)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>26.850369134350696</t>
+          <t>6235.631352941178</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>24.404313069295494</t>
+          <t>6235.631352941178</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>24.404313069295494</t>
+          <t>6235.631352941178</t>
         </is>
       </c>
       <c r="S19" t="n">
-        <v>97.92462640224433</v>
+        <v>96.84321809654125</v>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>120.66291505711594</t>
+          <t>88.81700000000002</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>107.26104386673909</t>
+          <t>88.81700000000002</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>97.74229126442023</t>
+          <t>88.81700000000002</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>05/04/2021 00:51:11</t>
+          <t>05/05/2021 02:16:00</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>0.3333</v>
       </c>
       <c r="C20" t="n">
-        <v>12.298</v>
+        <v>14.32</v>
       </c>
       <c r="D20" t="n">
-        <v>8.285</v>
+        <v>12.916</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -2190,89 +2185,89 @@
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>50.33554097072978</v>
+        <v>66.344829023523</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>14.68881595236873</t>
+          <t>15.450692188801574</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>21.744517656241968</t>
+          <t>24.744319551163485</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>25.212378142707124</t>
+          <t>24.744319551163485</t>
         </is>
       </c>
       <c r="N20" t="n">
-        <v>99.6711169645525</v>
+        <v>-185.5570084552775</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>(0, 0, 1)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>14.669617253847195</t>
+          <t>5890.118055555555</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>23.252071591878288</t>
+          <t>5890.118055555555</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>23.252071591878288</t>
+          <t>5890.118055555555</t>
         </is>
       </c>
       <c r="S20" t="n">
-        <v>97.50214910913863</v>
+        <v>96.06044627916</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>34.010624245757874</t>
+          <t>84.72894444444441</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>46.200888046383376</t>
+          <t>84.72894444444441</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>53.24545683308382</t>
+          <t>84.72894444444441</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>05/04/2021 00:52:20</t>
+          <t>05/05/2021 02:17:04</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.3390000000000001</v>
+        <v>0.3333</v>
       </c>
       <c r="C21" t="n">
-        <v>18.508</v>
+        <v>14.09</v>
       </c>
       <c r="D21" t="n">
-        <v>19.449</v>
+        <v>12.864</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -2281,89 +2276,89 @@
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>45.00639354217083</v>
+        <v>60.76242200745884</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>13.069798347357835</t>
+          <t>13.505878030510178</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>19.702683913173328</t>
+          <t>23.451845688336522</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>23.15694345369533</t>
+          <t>23.451845688336522</t>
         </is>
       </c>
       <c r="N21" t="n">
-        <v>99.07811655801038</v>
+        <v>-241.9838986830596</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>23.67171036543244</t>
+          <t>5580.865530459328</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>29.35822431056914</t>
+          <t>5580.865530459328</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>23.357406145817077</t>
+          <t>5580.865530459328</t>
         </is>
       </c>
       <c r="S21" t="n">
-        <v>97.44061810501177</v>
+        <v>95.3699713783754</v>
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>28.505396667832443</t>
+          <t>80.94931578947373</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>40.723523106371466</t>
+          <t>80.94931578947373</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>48.10629685312056</t>
+          <t>80.94931578947373</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>05/04/2021 00:53:29</t>
+          <t>05/05/2021 02:18:07</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.3333</v>
+        <v>0.4918</v>
       </c>
       <c r="C22" t="n">
-        <v>14.218</v>
+        <v>16.332</v>
       </c>
       <c r="D22" t="n">
-        <v>12.964</v>
+        <v>15.361</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -2372,89 +2367,89 @@
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>47.57984187596441</v>
+        <v>62.31778110715422</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>11.800826395167283</t>
+          <t>13.669436014890254</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>18.03555540871433</t>
+          <t>22.366704900744857</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>21.426973541583198</t>
+          <t>22.366704900744857</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>99.10163518255047</v>
+        <v>-239.694786179296</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>24.650236348521407</t>
+          <t>5302.526749999999</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>22.008494439321577</t>
+          <t>5302.526749999999</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>12.939328496403691</t>
+          <t>5302.526749999999</t>
         </is>
       </c>
       <c r="S22" t="n">
-        <v>97.55403790482985</v>
+        <v>95.44270280582784</v>
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>34.380832607893964</t>
+          <t>77.54504999999997</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>43.55152765657149</t>
+          <t>77.54504999999997</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>49.18390044592198</t>
+          <t>77.54504999999997</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>05/04/2021 00:54:38</t>
+          <t>05/05/2021 02:19:12</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.3333</v>
+        <v>0.3390000000000001</v>
       </c>
       <c r="C23" t="n">
-        <v>14.128</v>
+        <v>15.668</v>
       </c>
       <c r="D23" t="n">
-        <v>12.888</v>
+        <v>13.726</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -2463,89 +2458,89 @@
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>65.71017075218487</v>
+        <v>57.91502480044706</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>10.76823851232573</t>
+          <t>12.480088674314782</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>16.641521343970034</t>
+          <t>21.335427016127298</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>19.94728602861497</t>
+          <t>21.335427016127298</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>99.14208107184037</v>
+        <v>-279.7403421417946</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>10.543365230387542</t>
+          <t>5050.803190476188</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>7.948628633240233</t>
+          <t>5050.803190476188</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>8.431697992370935</t>
+          <t>5050.803190476188</t>
         </is>
       </c>
       <c r="S23" t="n">
-        <v>98.00211513789493</v>
+        <v>95.00056139684797</v>
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>28.685688357988084</t>
+          <t>74.58390476190473</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>38.59142276698823</t>
+          <t>74.58390476190473</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>44.83271008596715</t>
+          <t>74.58390476190473</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>05/04/2021 00:55:46</t>
+          <t>05/05/2021 02:20:16</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.3390000000000001</v>
+        <v>30.50850000000001</v>
       </c>
       <c r="C24" t="n">
-        <v>15.404</v>
+        <v>12.683</v>
       </c>
       <c r="D24" t="n">
-        <v>13.63</v>
+        <v>9.776</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -2554,89 +2549,89 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>62.29384553886161</v>
+        <v>65.66377025002483</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>9.916747002476912</t>
+          <t>12.226067647835604</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>15.461541499109169</t>
+          <t>20.419152925859365</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>18.669650857040313</t>
+          <t>20.419152925859365</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>99.26192403299321</v>
+        <v>-293.7949183812499</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>12.00371495576783</t>
+          <t>4821.93340909091</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>10.701099935026253</t>
+          <t>4821.93340909091</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>13.107609483731663</t>
+          <t>4821.93340909091</t>
         </is>
       </c>
       <c r="S24" t="n">
-        <v>97.9367868179899</v>
+        <v>94.58972877158482</v>
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>27.39949299672429</t>
+          <t>71.81763636363635</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>36.723482004437365</t>
+          <t>71.81763636363635</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>42.71437288214227</t>
+          <t>71.81763636363635</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>05/04/2021 00:56:56</t>
+          <t>05/05/2021 02:21:21</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.3390000000000001</v>
+        <v>38.5</v>
       </c>
       <c r="C25" t="n">
-        <v>15.404</v>
+        <v>19.073</v>
       </c>
       <c r="D25" t="n">
-        <v>13.63</v>
+        <v>63.891</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -2645,89 +2640,89 @@
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>63.57799805091729</v>
+        <v>69.46635556799299</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>9.203437048044048</t>
+          <t>34.15096730192247</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>14.450383184618751</t>
+          <t>21.73306593655211</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>17.55610141702369</t>
+          <t>21.73306593655211</t>
         </is>
       </c>
       <c r="N25" t="n">
-        <v>99.3366604626986</v>
+        <v>-276.8012163296692</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>14.39583747286357</t>
+          <t>4612.8355652173905</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>14.992697332029888</t>
+          <t>4612.8355652173905</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>14.970912645125448</t>
+          <t>4612.8355652173905</t>
         </is>
       </c>
       <c r="S25" t="n">
-        <v>98.05796814903627</v>
+        <v>95.18177610418014</v>
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>26.886281791339428</t>
+          <t>69.12017391304347</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>35.53833274259232</t>
+          <t>69.12017391304347</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
         <is>
-          <t>41.18531481806254</t>
+          <t>69.12017391304347</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>05/04/2021 00:58:08</t>
+          <t>05/05/2021 02:21:31</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.3333</v>
+        <v>38.5</v>
       </c>
       <c r="C26" t="n">
-        <v>13.954</v>
+        <v>19.073</v>
       </c>
       <c r="D26" t="n">
-        <v>12.864</v>
+        <v>63.891</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -2736,89 +2731,89 @@
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>38.15517152952012</v>
+        <v>72.98919116905763</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>0.33958006027560883</t>
+          <t>24.94753288255315</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>0.33889082408658405</t>
+          <t>22.02554236907236</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>0.3386547569016906</t>
+          <t>22.02554236907236</t>
         </is>
       </c>
       <c r="N26" t="n">
-        <v>99.37301686951157</v>
+        <v>-248.0286525598096</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>16.040601120416003</t>
+          <t>4421.428791666668</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>15.545491296734495</t>
+          <t>4421.428791666668</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>15.184267053162321</t>
+          <t>4421.428791666668</t>
         </is>
       </c>
       <c r="S26" t="n">
-        <v>98.00536732951186</v>
+        <v>95.91108987974042</v>
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>26.010585595720237</t>
+          <t>68.90228941187308</t>
         </is>
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>34.20201636013542</t>
+          <t>68.90228941187308</t>
         </is>
       </c>
       <c r="W26" t="inlineStr">
         <is>
-          <t>39.62175498634407</t>
+          <t>68.90228941187308</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>05/04/2021 00:59:19</t>
+          <t>05/05/2021 02:21:40</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.3279</v>
+        <v>38.5</v>
       </c>
       <c r="C27" t="n">
-        <v>14.086</v>
+        <v>19.073</v>
       </c>
       <c r="D27" t="n">
-        <v>12.864</v>
+        <v>63.891</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -2827,89 +2822,89 @@
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>38.21300924537</v>
+        <v>78.72106510954731</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>0.3346692057312503</t>
+          <t>32.12169982323222</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>0.33303089008538805</t>
+          <t>22.926578832228664</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>0.33383099685802053</t>
+          <t>22.926578832228664</t>
         </is>
       </c>
       <c r="N27" t="n">
-        <v>99.40428786940703</v>
+        <v>-222.4766905774392</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>13.354422671658785</t>
+          <t>4245.334560000001</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>13.984605616492141</t>
+          <t>4245.334560000001</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>14.346364592039482</t>
+          <t>4245.334560000001</t>
         </is>
       </c>
       <c r="S27" t="n">
-        <v>97.92057968103161</v>
+        <v>96.58361186308137</v>
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>24.69051112134136</t>
+          <t>68.70184</t>
         </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>32.6131947933644</t>
+          <t>68.70184</t>
         </is>
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>37.92067016990819</t>
+          <t>68.70184</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>05/04/2021 01:00:29</t>
+          <t>05/05/2021 02:21:48</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.3333</v>
+        <v>38.5</v>
       </c>
       <c r="C28" t="n">
-        <v>16.262</v>
+        <v>19.073</v>
       </c>
       <c r="D28" t="n">
-        <v>15.421</v>
+        <v>63.891</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -2918,89 +2913,89 @@
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>44.39029540892233</v>
+        <v>80.82073339848111</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>0.3285907646017213</t>
+          <t>27.633297957081528</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>0.32794970556482445</t>
+          <t>23.3245633482581</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>0.32875645035653317</t>
+          <t>23.3245633482581</t>
         </is>
       </c>
       <c r="N28" t="n">
-        <v>99.45463941837777</v>
+        <v>-211.5351245892781</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>14.762698225918793</t>
+          <t>4082.7860384615374</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>14.777512393623383</t>
+          <t>4082.7860384615374</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>14.516516226083633</t>
+          <t>4082.7860384615374</t>
         </is>
       </c>
       <c r="S28" t="n">
-        <v>98.07289472359096</v>
+        <v>96.91801052136432</v>
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>23.99923802573303</t>
+          <t>68.51680769230765</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>31.538621831587907</t>
+          <t>68.51680769230765</t>
         </is>
       </c>
       <c r="W28" t="inlineStr">
         <is>
-          <t>36.64334505713789</t>
+          <t>68.51680769230765</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>05/04/2021 01:01:42</t>
+          <t>05/05/2021 02:21:58</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.5</v>
+        <v>59.3443</v>
       </c>
       <c r="C29" t="n">
-        <v>16.262</v>
+        <v>20.152</v>
       </c>
       <c r="D29" t="n">
-        <v>15.421</v>
+        <v>113.958</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -3009,89 +3004,89 @@
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>78.62278329154269</v>
+        <v>85.05298826091415</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 1)</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>0.331082923687036</t>
+          <t>31.42638723073942</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>0.332934014081999</t>
+          <t>23.995479630906196</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>0.3318228460497261</t>
+          <t>23.995479630906196</t>
         </is>
       </c>
       <c r="N29" t="n">
-        <v>99.73221437430995</v>
+        <v>-193.0075170021011</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>16.36625014021729</t>
+          <t>3932.2781481481484</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>15.38692829303763</t>
+          <t>3932.2781481481484</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>15.34084085783632</t>
+          <t>3932.2781481481484</t>
         </is>
       </c>
       <c r="S29" t="n">
-        <v>98.84328295955487</v>
+        <v>97.36107959430724</v>
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>(1, 0, 0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>25.263373852647</t>
+          <t>68.34548148148149</t>
         </is>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>31.977954363585923</t>
+          <t>68.34548148148149</t>
         </is>
       </c>
       <c r="W29" t="inlineStr">
         <is>
-          <t>36.558718324889384</t>
+          <t>68.34548148148149</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>05/04/2021 01:02:51</t>
+          <t>05/05/2021 02:22:08</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.5</v>
+        <v>59.3443</v>
       </c>
       <c r="C30" t="n">
-        <v>16.19</v>
+        <v>20.152</v>
       </c>
       <c r="D30" t="n">
-        <v>15.232</v>
+        <v>113.958</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -3100,89 +3095,89 @@
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>92.72132365621924</v>
+        <v>92.03350087289022</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(1, 0, 1)</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>0.44380314112506486</t>
+          <t>51.49631064634037</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>0.4791493865269336</t>
+          <t>34.86104600076293</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>0.45012213863570105</t>
+          <t>29.07169617749027</t>
         </is>
       </c>
       <c r="N30" t="n">
-        <v>99.80907096288794</v>
+        <v>-170.6951742354552</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>15.27421286926913</t>
+          <t>3792.559357142857</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>15.277674108127478</t>
+          <t>3792.559357142857</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>15.760108345706522</t>
+          <t>3792.559357142857</t>
         </is>
       </c>
       <c r="S30" t="n">
-        <v>98.67181009853212</v>
+        <v>97.87848323666073</v>
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>14.497021556206562</t>
+          <t>69.97449999999999</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>14.215219349010326</t>
+          <t>69.97449999999999</t>
         </is>
       </c>
       <c r="W30" t="inlineStr">
         <is>
-          <t>15.178919621935126</t>
+          <t>69.97449999999999</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>05/04/2021 01:04:06</t>
+          <t>05/05/2021 02:22:18</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.3279</v>
+        <v>59.3443</v>
       </c>
       <c r="C31" t="n">
-        <v>14.02</v>
+        <v>20.152</v>
       </c>
       <c r="D31" t="n">
-        <v>12.864</v>
+        <v>113.958</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -3191,89 +3186,89 @@
         <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>93.33087516110608</v>
+        <v>92.73175952033495</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(1, 0, 1)</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>0.5159866501494</t>
+          <t>42.39236301815872</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>0.4989691441246671</t>
+          <t>32.36554331913829</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>0.498960476919359</t>
+          <t>28.69777544193331</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>99.81200044807562</v>
+        <v>-162.5176650941775</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>16.245039894668587</t>
+          <t>3662.4763448275844</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>16.285068204549408</t>
+          <t>3662.4763448275844</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>16.681768191348265</t>
+          <t>3662.4763448275844</t>
         </is>
       </c>
       <c r="S31" t="n">
-        <v>98.77760007903896</v>
+        <v>98.03747082198355</v>
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>14.980129490842732</t>
+          <t>71.49117241379307</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>15.748747580445214</t>
+          <t>71.49117241379307</t>
         </is>
       </c>
       <c r="W31" t="inlineStr">
         <is>
-          <t>15.450699587425797</t>
+          <t>71.49117241379307</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>05/04/2021 01:05:18</t>
+          <t>05/05/2021 02:22:30</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.3390000000000001</v>
+        <v>59.3443</v>
       </c>
       <c r="C32" t="n">
-        <v>17.773</v>
+        <v>20.152</v>
       </c>
       <c r="D32" t="n">
-        <v>16.578</v>
+        <v>113.958</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -3282,89 +3277,89 @@
         <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>94.37423026530031</v>
+        <v>95.54632298508412</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(1, 0, 1)</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>0.3761249912651896</t>
+          <t>48.665787606897</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>0.3356303231997302</t>
+          <t>36.60834836127581</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>0.36907775130861853</t>
+          <t>31.54907780252605</t>
         </is>
       </c>
       <c r="N32" t="n">
-        <v>99.81775691641801</v>
+        <v>-142.4841053200366</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>13.939760605744368</t>
+          <t>3541.065533333333</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>15.417402184287939</t>
+          <t>3541.065533333333</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>15.312097794631974</t>
+          <t>3541.065533333333</t>
         </is>
       </c>
       <c r="S32" t="n">
-        <v>99.15665655136868</v>
+        <v>98.48587720742191</v>
       </c>
       <c r="T32" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>13.549150906497038</t>
+          <t>72.9067333333333</t>
         </is>
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>13.823688174009444</t>
+          <t>72.9067333333333</t>
         </is>
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>14.010475258305732</t>
+          <t>72.9067333333333</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05/04/2021 01:06:29</t>
+          <t>05/05/2021 02:22:40</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.3390000000000001</v>
+        <v>59.3443</v>
       </c>
       <c r="C33" t="n">
-        <v>15.728</v>
+        <v>20.152</v>
       </c>
       <c r="D33" t="n">
-        <v>13.978</v>
+        <v>113.958</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -3373,89 +3368,89 @@
         <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>97.59282098520771</v>
+        <v>97.30772810253534</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(1, 0, 1)</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>0.3113630508982408</t>
+          <t>46.99167805480859</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>0.33693740743434675</t>
+          <t>36.645170411857066</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>0.34085267586640666</t>
+          <t>32.157482837756234</t>
         </is>
       </c>
       <c r="N33" t="n">
-        <v>99.86310521443079</v>
+        <v>-128.4305383948728</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>19.4225570188839</t>
+          <t>3427.4876774193563</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>17.45812290986296</t>
+          <t>3427.4876774193563</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>17.127889435019764</t>
+          <t>3427.4876774193563</t>
         </is>
       </c>
       <c r="S33" t="n">
-        <v>99.25692071575236</v>
+        <v>98.82220139171311</v>
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>16.970159859759885</t>
+          <t>74.2309677419355</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>16.32958630790219</t>
+          <t>74.2309677419355</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
         <is>
-          <t>15.061873928522015</t>
+          <t>74.2309677419355</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>05/04/2021 01:07:40</t>
+          <t>05/05/2021 02:22:49</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.3333</v>
+        <v>83.5</v>
       </c>
       <c r="C34" t="n">
-        <v>14.392</v>
+        <v>20.152</v>
       </c>
       <c r="D34" t="n">
-        <v>12.892</v>
+        <v>115.033</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -3464,1594 +3459,72 @@
         <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>97.78801050341256</v>
+        <v>97.99788335533144</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(1, 0, 0)</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>0.3549327686181057</t>
+          <t>50.76518576884423</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>0.36480390321430234</t>
+          <t>44.66896476812417</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>0.3674347303293458</t>
+          <t>40.33705945852279</t>
         </is>
       </c>
       <c r="N34" t="n">
-        <v>99.87027991678153</v>
+        <v>-123.0444899785308</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>13.660910040868863</t>
+          <t>3321.0084375000006</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>15.098085485300416</t>
+          <t>3321.0084375000006</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>15.537625507347071</t>
+          <t>3321.0084375000006</t>
         </is>
       </c>
       <c r="S34" t="n">
-        <v>99.31669674217653</v>
+        <v>98.89169242530569</v>
       </c>
       <c r="T34" t="inlineStr">
         <is>
-          <t>(5,1,0)</t>
+          <t>(0, 0, 0)</t>
         </is>
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>13.224187740595646</t>
+          <t>75.47243750000001</t>
         </is>
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>12.775238495988347</t>
+          <t>75.47243750000001</t>
         </is>
       </c>
       <c r="W34" t="inlineStr">
         <is>
-          <t>14.893970793903495</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:08:53</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>0.3333</v>
-      </c>
-      <c r="C35" t="n">
-        <v>14.392</v>
-      </c>
-      <c r="D35" t="n">
-        <v>12.892</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" t="n">
-        <v>99.39828144724903</v>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>0.3508350983529307</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>0.3488342795538077</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>0.3511365736515818</t>
-        </is>
-      </c>
-      <c r="N35" t="n">
-        <v>99.88301535187169</v>
-      </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t>15.844157736723751</t>
-        </is>
-      </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>15.934586603998643</t>
-        </is>
-      </c>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>15.794108523687122</t>
-        </is>
-      </c>
-      <c r="S35" t="n">
-        <v>99.64152673782117</v>
-      </c>
-      <c r="T35" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>12.42866449580328</t>
-        </is>
-      </c>
-      <c r="V35" t="inlineStr">
-        <is>
-          <t>14.645673030671055</t>
-        </is>
-      </c>
-      <c r="W35" t="inlineStr">
-        <is>
-          <t>13.616610481001981</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:12:26</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>0.3333</v>
-      </c>
-      <c r="C36" t="n">
-        <v>17.144</v>
-      </c>
-      <c r="D36" t="n">
-        <v>17.13</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:12:53</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>0.3333</v>
-      </c>
-      <c r="C37" t="n">
-        <v>17.144</v>
-      </c>
-      <c r="D37" t="n">
-        <v>17.13</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" t="n">
-        <v>99.89191175971352</v>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>0.33332927071827945</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>0.3335945120700176</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>0.33341800718902725</t>
-        </is>
-      </c>
-      <c r="N37" t="n">
-        <v>99.89426485663127</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P37" t="inlineStr">
-        <is>
-          <t>17.74197857000672</t>
-        </is>
-      </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>16.167071932293275</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>15.9300597461864</t>
-        </is>
-      </c>
-      <c r="S37" t="n">
-        <v>99.87001812282764</v>
-      </c>
-      <c r="T37" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>16.03303136905383</t>
-        </is>
-      </c>
-      <c r="V37" t="inlineStr">
-        <is>
-          <t>15.022237889284888</t>
-        </is>
-      </c>
-      <c r="W37" t="inlineStr">
-        <is>
-          <t>14.839831390124328</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:14:17</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>0.3390000000000001</v>
-      </c>
-      <c r="C38" t="n">
-        <v>14.615</v>
-      </c>
-      <c r="D38" t="n">
-        <v>13.499</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" t="n">
-        <v>99.89117478491096</v>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>0.33358442994273724</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>0.33340599129966386</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>0.3332310873142399</t>
-        </is>
-      </c>
-      <c r="N38" t="n">
-        <v>99.89435781042539</v>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t>15.553863220392229</t>
-        </is>
-      </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>15.604859185258828</t>
-        </is>
-      </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>16.390277008404002</t>
-        </is>
-      </c>
-      <c r="S38" t="n">
-        <v>99.88239561293616</v>
-      </c>
-      <c r="T38" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>16.15550010612316</t>
-        </is>
-      </c>
-      <c r="V38" t="inlineStr">
-        <is>
-          <t>15.664138921658818</t>
-        </is>
-      </c>
-      <c r="W38" t="inlineStr">
-        <is>
-          <t>17.142681632215368</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:16:06</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>0.1695</v>
-      </c>
-      <c r="C39" t="n">
-        <v>15.224</v>
-      </c>
-      <c r="D39" t="n">
-        <v>13.526</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" t="n">
-        <v>99.81666216103642</v>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>0.3368822967307062</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>0.3378560768180468</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>0.3366162091934315</t>
-        </is>
-      </c>
-      <c r="N39" t="n">
-        <v>99.9029317070418</v>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t>14.644367391398882</t>
-        </is>
-      </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>15.886288687437649</t>
-        </is>
-      </c>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>16.14501321664819</t>
-        </is>
-      </c>
-      <c r="S39" t="n">
-        <v>99.89836111328113</v>
-      </c>
-      <c r="T39" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>12.918782582145148</t>
-        </is>
-      </c>
-      <c r="V39" t="inlineStr">
-        <is>
-          <t>15.151005589615048</t>
-        </is>
-      </c>
-      <c r="W39" t="inlineStr">
-        <is>
-          <t>15.217691566882445</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:17:23</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>0.3390000000000001</v>
-      </c>
-      <c r="C40" t="n">
-        <v>14.67</v>
-      </c>
-      <c r="D40" t="n">
-        <v>13.586</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" t="n">
-        <v>99.80687930228349</v>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>0.23041902494994412</t>
-        </is>
-      </c>
-      <c r="L40" t="inlineStr">
-        <is>
-          <t>0.19359000768430448</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>0.22493600508240605</t>
-        </is>
-      </c>
-      <c r="N40" t="n">
-        <v>99.90105176644022</v>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P40" t="inlineStr">
-        <is>
-          <t>16.480094058449186</t>
-        </is>
-      </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>16.456679992046784</t>
-        </is>
-      </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>15.98796754870144</t>
-        </is>
-      </c>
-      <c r="S40" t="n">
-        <v>99.89407679248627</v>
-      </c>
-      <c r="T40" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U40" t="inlineStr">
-        <is>
-          <t>15.781760867426108</t>
-        </is>
-      </c>
-      <c r="V40" t="inlineStr">
-        <is>
-          <t>15.675105526268911</t>
-        </is>
-      </c>
-      <c r="W40" t="inlineStr">
-        <is>
-          <t>14.085281008538876</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:18:35</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>0.3333</v>
-      </c>
-      <c r="C41" t="n">
-        <v>14.67</v>
-      </c>
-      <c r="D41" t="n">
-        <v>13.586</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="n">
-        <v>99.79332114858366</v>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>0.263154259246667</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>0.3176264360155145</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>0.28756440565843094</t>
-        </is>
-      </c>
-      <c r="N41" t="n">
-        <v>99.90447574017222</v>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P41" t="inlineStr">
-        <is>
-          <t>14.611307489469578</t>
-        </is>
-      </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>15.025501936099918</t>
-        </is>
-      </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>14.629713950990197</t>
-        </is>
-      </c>
-      <c r="S41" t="n">
-        <v>99.89910055198395</v>
-      </c>
-      <c r="T41" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U41" t="inlineStr">
-        <is>
-          <t>13.409114557433316</t>
-        </is>
-      </c>
-      <c r="V41" t="inlineStr">
-        <is>
-          <t>12.442429537762328</t>
-        </is>
-      </c>
-      <c r="W41" t="inlineStr">
-        <is>
-          <t>13.198534488186723</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:19:47</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>0.3333</v>
-      </c>
-      <c r="C42" t="n">
-        <v>13.504</v>
-      </c>
-      <c r="D42" t="n">
-        <v>12.484</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" t="n">
-        <v>99.78805345713816</v>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>0.36258933722128595</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>0.3473835103953428</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>0.3447241548034348</t>
-        </is>
-      </c>
-      <c r="N42" t="n">
-        <v>99.90269355584674</v>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>15.085956078353899</t>
-        </is>
-      </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>14.660321956101058</t>
-        </is>
-      </c>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>14.566165518103134</t>
-        </is>
-      </c>
-      <c r="S42" t="n">
-        <v>99.90832391061794</v>
-      </c>
-      <c r="T42" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U42" t="inlineStr">
-        <is>
-          <t>12.622716043680835</t>
-        </is>
-      </c>
-      <c r="V42" t="inlineStr">
-        <is>
-          <t>13.33027075802675</t>
-        </is>
-      </c>
-      <c r="W42" t="inlineStr">
-        <is>
-          <t>13.632404170104312</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:21:01</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>0.3333</v>
-      </c>
-      <c r="C43" t="n">
-        <v>15.006</v>
-      </c>
-      <c r="D43" t="n">
-        <v>13.914</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" t="n">
-        <v>99.80125380303248</v>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>0.328653346562816</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>0.31976128052061636</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>0.3171299966115185</t>
-        </is>
-      </c>
-      <c r="N43" t="n">
-        <v>99.90049597406974</v>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>13.051165816849764</t>
-        </is>
-      </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>13.723458211277789</t>
-        </is>
-      </c>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>13.761439256901982</t>
-        </is>
-      </c>
-      <c r="S43" t="n">
-        <v>99.91096353731902</v>
-      </c>
-      <c r="T43" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>13.189335381120046</t>
-        </is>
-      </c>
-      <c r="V43" t="inlineStr">
-        <is>
-          <t>13.531629544577722</t>
-        </is>
-      </c>
-      <c r="W43" t="inlineStr">
-        <is>
-          <t>13.496334873830415</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:22:16</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>0.3390000000000001</v>
-      </c>
-      <c r="C44" t="n">
-        <v>13.612</v>
-      </c>
-      <c r="D44" t="n">
-        <v>12.612</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" t="n">
-        <v>99.82057207489673</v>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>0.32270763468952146</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>0.3210569798981176</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>0.3207920592362488</t>
-        </is>
-      </c>
-      <c r="N44" t="n">
-        <v>99.890662622143</v>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t>15.70703568968809</t>
-        </is>
-      </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>14.800130091904405</t>
-        </is>
-      </c>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>14.590676395294604</t>
-        </is>
-      </c>
-      <c r="S44" t="n">
-        <v>99.90243143124786</v>
-      </c>
-      <c r="T44" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U44" t="inlineStr">
-        <is>
-          <t>14.277968683939081</t>
-        </is>
-      </c>
-      <c r="V44" t="inlineStr">
-        <is>
-          <t>14.03412445072183</t>
-        </is>
-      </c>
-      <c r="W44" t="inlineStr">
-        <is>
-          <t>13.364099929296813</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:25:09</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>43.0508</v>
-      </c>
-      <c r="C45" t="n">
-        <v>202.381</v>
-      </c>
-      <c r="D45" t="n">
-        <v>254.791</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" t="n">
-        <v>99.76191152388162</v>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>0.3314057912712764</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>0.33458016451216516</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>0.3321060736934448</t>
-        </is>
-      </c>
-      <c r="N45" t="n">
-        <v>99.83194459722796</v>
-      </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P45" t="inlineStr">
-        <is>
-          <t>12.682132470960529</t>
-        </is>
-      </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>13.486923682015501</t>
-        </is>
-      </c>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>13.623827604966296</t>
-        </is>
-      </c>
-      <c r="S45" t="n">
-        <v>99.84220518133121</v>
-      </c>
-      <c r="T45" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t>12.32016145887991</t>
-        </is>
-      </c>
-      <c r="V45" t="inlineStr">
-        <is>
-          <t>12.130174310140573</t>
-        </is>
-      </c>
-      <c r="W45" t="inlineStr">
-        <is>
-          <t>13.023648545079404</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:26:26</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>83.33329999999999</v>
-      </c>
-      <c r="C46" t="n">
-        <v>24.282</v>
-      </c>
-      <c r="D46" t="n">
-        <v>111.143</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" t="n">
-        <v>99.73497402850202</v>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>27.57595545362523</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>36.552700621925275</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>28.42757126884946</t>
-        </is>
-      </c>
-      <c r="N46" t="n">
-        <v>99.45505373821773</v>
-      </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t>174.78934270589156</t>
-        </is>
-      </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>148.63744192669824</t>
-        </is>
-      </c>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>142.13820880671352</t>
-        </is>
-      </c>
-      <c r="S46" t="n">
-        <v>99.76913404929236</v>
-      </c>
-      <c r="T46" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U46" t="inlineStr">
-        <is>
-          <t>258.62230678240434</t>
-        </is>
-      </c>
-      <c r="V46" t="inlineStr">
-        <is>
-          <t>194.90768868455248</t>
-        </is>
-      </c>
-      <c r="W46" t="inlineStr">
-        <is>
-          <t>155.4874102055009</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:31:48</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>11.6102</v>
-      </c>
-      <c r="C47" t="n">
-        <v>58.3</v>
-      </c>
-      <c r="D47" t="n">
-        <v>70.202</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" t="n">
-        <v>99.39642166050268</v>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>81.16049563129052</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>82.96279050996131</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>76.32865128433885</t>
-        </is>
-      </c>
-      <c r="N47" t="n">
-        <v>99.42551172475147</v>
-      </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>95.10927417410173</t>
-        </is>
-      </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>62.21687476445978</t>
-        </is>
-      </c>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>98.99839781612866</t>
-        </is>
-      </c>
-      <c r="S47" t="n">
-        <v>99.76158800314099</v>
-      </c>
-      <c r="T47" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>90.22619764659858</t>
-        </is>
-      </c>
-      <c r="V47" t="inlineStr">
-        <is>
-          <t>86.35595336799152</t>
-        </is>
-      </c>
-      <c r="W47" t="inlineStr">
-        <is>
-          <t>176.39517846173285</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:37:10</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>0.3390000000000001</v>
-      </c>
-      <c r="C48" t="n">
-        <v>14.434</v>
-      </c>
-      <c r="D48" t="n">
-        <v>13.048</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="I48" t="n">
-        <v>93.92508572044355</v>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>30.052651130145946</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>22.131959387201633</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>31.009610750216204</t>
-        </is>
-      </c>
-      <c r="N48" t="n">
-        <v>99.19587926753739</v>
-      </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>70.57932982191049</t>
-        </is>
-      </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>85.08358228776439</t>
-        </is>
-      </c>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>77.46469221921265</t>
-        </is>
-      </c>
-      <c r="S48" t="n">
-        <v>99.46510396890004</v>
-      </c>
-      <c r="T48" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>77.32828662805731</t>
-        </is>
-      </c>
-      <c r="V48" t="inlineStr">
-        <is>
-          <t>169.05331110729134</t>
-        </is>
-      </c>
-      <c r="W48" t="inlineStr">
-        <is>
-          <t>108.2074385178062</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:39:40</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>0.3333</v>
-      </c>
-      <c r="C49" t="n">
-        <v>14.104</v>
-      </c>
-      <c r="D49" t="n">
-        <v>12.932</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" t="n">
-        <v>93.7690786731073</v>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>3.24202046028808</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>17.777327533373818</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>21.022165795019955</t>
-        </is>
-      </c>
-      <c r="N49" t="n">
-        <v>98.89447445188235</v>
-      </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>97.71254865063152</t>
-        </is>
-      </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>71.45316841977734</t>
-        </is>
-      </c>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>78.72293785152937</t>
-        </is>
-      </c>
-      <c r="S49" t="n">
-        <v>98.90783204547526</v>
-      </c>
-      <c r="T49" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U49" t="inlineStr">
-        <is>
-          <t>142.36216420758166</t>
-        </is>
-      </c>
-      <c r="V49" t="inlineStr">
-        <is>
-          <t>87.79255348737931</t>
-        </is>
-      </c>
-      <c r="W49" t="inlineStr">
-        <is>
-          <t>99.38424556569488</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:49:48</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>0.3448</v>
-      </c>
-      <c r="C50" t="n">
-        <v>14.214</v>
-      </c>
-      <c r="D50" t="n">
-        <v>12.812</v>
-      </c>
-      <c r="E50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I50" t="n">
-        <v>91.14870243958147</v>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>15.732507124093702</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>19.77711404241292</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>21.06583695360908</t>
-        </is>
-      </c>
-      <c r="N50" t="n">
-        <v>98.58458613092358</v>
-      </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>92.43370772307951</t>
-        </is>
-      </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>74.15147609478524</t>
-        </is>
-      </c>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>64.20658650073828</t>
-        </is>
-      </c>
-      <c r="S50" t="n">
-        <v>98.84540504592096</v>
-      </c>
-      <c r="T50" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U50" t="inlineStr">
-        <is>
-          <t>29.15141367660464</t>
-        </is>
-      </c>
-      <c r="V50" t="inlineStr">
-        <is>
-          <t>64.01531968547494</t>
-        </is>
-      </c>
-      <c r="W50" t="inlineStr">
-        <is>
-          <t>58.35296318240156</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:50:44</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>0.3448</v>
-      </c>
-      <c r="C51" t="n">
-        <v>14.084</v>
-      </c>
-      <c r="D51" t="n">
-        <v>12.812</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:54:54</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>82.03389999999999</v>
-      </c>
-      <c r="C52" t="n">
-        <v>594715.41</v>
-      </c>
-      <c r="D52" t="n">
-        <v>963.941</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>05/04/2021 01:56:09</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>8.666700000000001</v>
-      </c>
-      <c r="C53" t="n">
-        <v>14.07</v>
-      </c>
-      <c r="D53" t="n">
-        <v>12.852</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0</v>
-      </c>
-      <c r="I53" t="n">
-        <v>89.87832261394433</v>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>57.78116281411748</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>50.94413659754122</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>39.414010215544096</t>
-        </is>
-      </c>
-      <c r="N53" t="n">
-        <v>53.48702673794435</v>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>(0, 0, 0)</t>
-        </is>
-      </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>11683.660725490196</t>
-        </is>
-      </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>11683.660725490196</t>
-        </is>
-      </c>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>11683.660725490196</t>
-        </is>
-      </c>
-      <c r="S53" t="n">
-        <v>96.15196511216485</v>
-      </c>
-      <c r="T53" t="inlineStr">
-        <is>
-          <t>(5,1,0)</t>
-        </is>
-      </c>
-      <c r="U53" t="inlineStr">
-        <is>
-          <t>595.6891021836261</t>
-        </is>
-      </c>
-      <c r="V53" t="inlineStr">
-        <is>
-          <t>383.54277254378417</t>
-        </is>
-      </c>
-      <c r="W53" t="inlineStr">
-        <is>
-          <t>291.1782290975657</t>
+          <t>75.47243750000001</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add median and percentile to get upper and lower threasholds
</commit_message>
<xml_diff>
--- a/dataset/all.xlsx
+++ b/dataset/all.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:BB2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,85 +451,105 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>instance</t>
+          <t>up_cpu</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>down_cpu</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>up_netin</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>down_netin</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>up_netout</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>down_netout</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
           <t>cpu_acc</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>cpu_model</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>cpu_pred1</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>cpu_pred2</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>cpu_pred3</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>netin_acc</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>netin_model</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>netin_pred1</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>netin_pred2</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>netin_pred3</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>netout_acc</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>netout_model</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>netout_pred1</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>netout_pred2</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>netout_pred3</t>
         </is>
@@ -538,14 +558,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>05/07/2021 03:17:51</t>
+          <t>05/08/2021 02:45:17</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5</v>
+        <v>0.3390000000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>14.084</v>
+        <v>14.368</v>
       </c>
       <c r="D2" t="n">
         <v>12.736</v>
@@ -553,71 +573,98 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="n">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.3390000000000001</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.3390000000000001</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>14.368</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>14.368</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>12.736</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>12.736</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>(0, 0, 0)</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
         <v>0</v>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>(0, 0, 0)</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N2" t="n">
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>(0, 0, 0)</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>(0, 0, 0)</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>